<commit_message>
v.2.0.0 - support cms v7
</commit_message>
<xml_diff>
--- a/assets/excel/products-demo-add.xlsx
+++ b/assets/excel/products-demo-add.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huutr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C763FC15-6064-46B7-BB31-0CBE0533027E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833ED73B-AE36-49A7-902D-C1C6BD5C1237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="60">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="62">
   <si>
     <t>Id Nhóm</t>
   </si>
@@ -200,6 +197,15 @@
   </si>
   <si>
     <t>SP223</t>
+  </si>
+  <si>
+    <t>Dài (cm)</t>
+  </si>
+  <si>
+    <t>Rộng (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cao (cm)</t>
   </si>
 </sst>
 </file>
@@ -577,31 +583,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16.28515625" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="25" max="25" width="21" customWidth="1"/>
+    <col min="26" max="26" width="35" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -625,13 +644,13 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>12</v>
@@ -643,543 +662,597 @@
         <v>14</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="N2" s="1">
+        <v>4190000</v>
+      </c>
       <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="1"/>
+    </row>
+    <row r="3" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1">
         <v>4190000</v>
       </c>
-      <c r="P2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X2" s="1" t="s">
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Y2" s="1"/>
+      <c r="AA3" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
         <v>4190000</v>
       </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y3" s="1"/>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA4" s="1"/>
     </row>
-    <row r="4" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1">
-        <v>4190000</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y4" s="1"/>
-    </row>
-    <row r="5" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1">
+        <v>4190000</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1">
-        <v>4190000</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="1">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y5" s="1"/>
-    </row>
-    <row r="6" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="N6" s="1">
+        <v>4190000</v>
+      </c>
       <c r="O6" s="1">
-        <v>4190000</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
       </c>
       <c r="R6" s="1">
         <v>0</v>
       </c>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1"/>
       <c r="V6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y6" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0</v>
+    <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="1">
+        <v>4190000</v>
+      </c>
       <c r="O7" s="1">
-        <v>4190000</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
       </c>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1"/>
       <c r="V7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y7" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0</v>
+    <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="1">
+        <v>4190000</v>
+      </c>
       <c r="O8" s="1">
-        <v>4190000</v>
-      </c>
-      <c r="P8" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
       </c>
       <c r="R8" s="1">
         <v>0</v>
       </c>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1"/>
       <c r="V8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y8" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1">
         <v>222</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="N9" s="1">
+        <v>4190000</v>
+      </c>
       <c r="O9" s="1">
-        <v>4190000</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
       </c>
       <c r="R9" s="1">
         <v>0</v>
       </c>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1"/>
       <c r="V9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y9" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA9" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>